<commit_message>
Lab 4 - Question 1 Done
</commit_message>
<xml_diff>
--- a/Lab3/ExecutionTime.xlsx
+++ b/Lab3/ExecutionTime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/805fd1da7aba8867/Documents/Universitet/Year 2/ID1021 Algoritmer och Datastrukturer/Lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{F9D85B67-9C5A-47A9-B46D-AE66EA5C1378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF59097B-FAC3-48D1-9101-394D3F066248}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{F9D85B67-9C5A-47A9-B46D-AE66EA5C1378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFAD8BBF-B9FD-4A09-8B82-C24B3A799BC9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{6355DACB-2D77-410C-9154-748C17C833A6}"/>
   </bookViews>
@@ -3894,8 +3894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A7D488-AB60-42BF-A09C-220C6A4BB5B7}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3908,9 +3908,9 @@
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.85546875" style="1" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" style="1" bestFit="1" customWidth="1"/>

</xml_diff>